<commit_message>
List of materials with price and where to buy
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rigorini\Documents\Diego\Progetti Hardware\3DWall\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rigorini\Documents\Diego\Progetti Hardware\Rigorini 3D Printer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2E68F14F-364D-472A-8AAE-5A2C0332082D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D53108F7-AAE8-4F9A-993D-A7F1B9958B5D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="9525" xr2:uid="{AD4B5A2A-0E8B-44A7-91E1-D202EB516C4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
   <si>
     <t>Description</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Relay 12V 40A</t>
+  </si>
+  <si>
+    <t>Local Car Parts Store</t>
+  </si>
+  <si>
+    <t>Ramps RRD Fan Extender</t>
   </si>
 </sst>
 </file>
@@ -350,10 +359,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB5A1A39-22B8-421A-A6D0-EB6DE4E4E595}" name="Tabella1" displayName="Tabella1" ref="A1:E62" totalsRowShown="0">
-  <autoFilter ref="A1:E62" xr:uid="{3E9E45AB-70B0-42EA-9702-5CDCA21C9473}"/>
-  <sortState ref="A2:E62">
-    <sortCondition ref="A1:A62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB5A1A39-22B8-421A-A6D0-EB6DE4E4E595}" name="Tabella1" displayName="Tabella1" ref="A1:E64" totalsRowShown="0">
+  <autoFilter ref="A1:E64" xr:uid="{3E9E45AB-70B0-42EA-9702-5CDCA21C9473}"/>
+  <sortState ref="A2:E64">
+    <sortCondition ref="A1:A64"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6B75AC82-E8F8-4AF9-9A78-CEA1F2759817}" name="Description"/>
@@ -663,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32797C51-70DD-4CCD-9DA5-A660F21D8FD8}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" ref="E34:E44" si="0">D34*B34</f>
+        <f t="shared" ref="E34:E46" si="0">D34*B34</f>
         <v>3</v>
       </c>
     </row>
@@ -1260,28 +1269,28 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B38" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D38" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B39" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
         <v>25</v>
@@ -1291,15 +1300,15 @@
       </c>
       <c r="E39" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B40" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
@@ -1309,12 +1318,12 @@
       </c>
       <c r="E40" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B41" s="4">
         <v>2</v>
@@ -1332,10 +1341,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -1345,73 +1354,87 @@
       </c>
       <c r="E42" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D43" s="2">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="E43" s="3">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="D44" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E44" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B45" s="4">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="D45" s="2">
+        <v>35</v>
+      </c>
+      <c r="E45" s="3">
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="D46" s="2">
+        <v>10</v>
+      </c>
+      <c r="E46" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B47" s="4">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C47" t="s">
         <v>25</v>
@@ -1419,10 +1442,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B48" s="4">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
         <v>25</v>
@@ -1430,99 +1453,98 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B49" s="4">
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="3">
-        <f>D49*B49</f>
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" s="4">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="2">
-        <v>2</v>
-      </c>
-      <c r="E50" s="3">
-        <f>D50*B50</f>
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B51" s="4">
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E51" s="3">
+        <f>D51*B51</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D52" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E52" s="3">
         <f>D52*B52</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="B53" s="4">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
         <v>25</v>
       </c>
+      <c r="E53" s="3"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B54" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="3"/>
+      <c r="D54" s="2">
+        <v>7</v>
+      </c>
+      <c r="E54" s="3">
+        <f>D54*B54</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B55" s="4">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C55" t="s">
         <v>25</v>
@@ -1530,21 +1552,22 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B56" s="4">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
       </c>
+      <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B57" s="4">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
@@ -1552,76 +1575,98 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B58" s="4">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
-      </c>
-      <c r="D58" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="E58" s="3">
-        <f>D58*B58</f>
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B59" s="4">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="2">
-        <v>5.3</v>
-      </c>
-      <c r="E59" s="3">
-        <f>D59*B59</f>
-        <v>10.6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C60" t="s">
         <v>64</v>
       </c>
       <c r="D60" s="2">
-        <v>3</v>
+        <v>7.5</v>
       </c>
       <c r="E60" s="3">
         <f>D60*B60</f>
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="4">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>64</v>
+      </c>
+      <c r="D61" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="E61" s="3">
+        <f>D61*B61</f>
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="2">
+        <v>3</v>
+      </c>
+      <c r="E62" s="3">
+        <f>D62*B62</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>63</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E63" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7">
-        <f>SUBTOTAL(109,E2:E61)</f>
-        <v>384.30000000000007</v>
+      <c r="B64" s="6"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7">
+        <f>SUBTOTAL(109,E2:E63)</f>
+        <v>392.30000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>